<commit_message>
Update peak LED trimmer in BOM.
</commit_message>
<xml_diff>
--- a/Modules/VU/VU_BOM.xlsx
+++ b/Modules/VU/VU_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\VU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3543EAD8-C76E-4635-AA94-454B0DC075B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CF0183-8206-44A6-8AF4-5DDE49FFC852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -362,16 +362,10 @@
     <t>https://www.thonk.co.uk/shop/tall-trimmer-toppers/</t>
   </si>
   <si>
-    <t>B10k</t>
-  </si>
-  <si>
     <t>6mm Trimpot</t>
   </si>
   <si>
     <t>Trimmer THT</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/hr/en/details/rkt6v-10k/single-turn-tht-trimmers/sr-passives/</t>
   </si>
   <si>
     <t>https://www.tme.eu/hr/en/details/rkt6v-100k/single-turn-tht-trimmers/sr-passives/</t>
@@ -541,6 +535,12 @@
       </rPr>
       <t>******</t>
     </r>
+  </si>
+  <si>
+    <t>B20k</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/hr/en/details/rkt6v-20k/single-turn-tht-trimmers/sr-passives/</t>
   </si>
 </sst>
 </file>
@@ -1459,7 +1459,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,7 +1584,7 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
@@ -1618,19 +1618,19 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" t="s">
         <v>105</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" t="s">
         <v>106</v>
       </c>
-      <c r="D8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" t="s">
-        <v>107</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1641,16 +1641,16 @@
         <v>93</v>
       </c>
       <c r="C9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" t="s">
         <v>106</v>
       </c>
-      <c r="D9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1721,7 +1721,7 @@
         <v>65</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D13" t="s">
         <v>67</v>
@@ -1838,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C19" t="s">
         <v>80</v>
@@ -1847,7 +1847,7 @@
         <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>77</v>
@@ -1984,7 +1984,7 @@
         <v>100</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E26" t="s">
         <v>26</v>
@@ -1995,13 +1995,13 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
         <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E27" t="s">
         <v>26</v>
@@ -2083,13 +2083,13 @@
         <v>46</v>
       </c>
       <c r="C33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="E33" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2110,27 +2110,27 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>